<commit_message>
finished test code for first batch of real project codes
</commit_message>
<xml_diff>
--- a/tests/RealProjectCode.xlsx
+++ b/tests/RealProjectCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\exaba\maxio-driver-demo\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC26BB04-A8B0-4F7B-93E3-07DFA07227F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D600B655-E520-4793-B958-0AE4359A040B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="39225" yWindow="0" windowWidth="24375" windowHeight="15330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
   <si>
     <t>Code</t>
   </si>
@@ -158,10 +158,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -504,8 +510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -677,6 +683,9 @@
       <c r="B14" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="C14" s="6" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="15" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
@@ -686,6 +695,9 @@
       <c r="B15" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="C15" s="6" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="16" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
@@ -695,8 +707,11 @@
       <c r="B16" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C16" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -704,8 +719,11 @@
       <c r="B17" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C17" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -713,8 +731,12 @@
       <c r="B18" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="C18" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update xlsx test results
</commit_message>
<xml_diff>
--- a/tests/RealProjectCode.xlsx
+++ b/tests/RealProjectCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\exaba\maxio-driver-demo\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D600B655-E520-4793-B958-0AE4359A040B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5793785-6308-45E5-BF38-1CD95CDE9EFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="39225" yWindow="0" windowWidth="24375" windowHeight="15330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
   <si>
     <t>Code</t>
   </si>
@@ -128,9 +128,6 @@
   </si>
   <si>
     <t>passed</t>
-  </si>
-  <si>
-    <t>Update is ok. Create failed test.</t>
   </si>
   <si>
     <t>failed</t>
@@ -205,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -217,16 +214,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -510,15 +504,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="3"/>
     <col min="2" max="2" width="97.33203125" customWidth="1"/>
-    <col min="3" max="3" width="31" style="5" customWidth="1"/>
+    <col min="3" max="3" width="31" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -528,7 +522,7 @@
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -539,7 +533,7 @@
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -551,7 +545,7 @@
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -563,7 +557,7 @@
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -575,7 +569,7 @@
       <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -587,7 +581,7 @@
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -599,7 +593,7 @@
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -611,7 +605,7 @@
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -623,7 +617,7 @@
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -635,8 +629,8 @@
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>20</v>
+      <c r="C10" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
@@ -647,8 +641,8 @@
       <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>21</v>
+      <c r="C11" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
@@ -657,10 +651,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="7" t="s">
         <v>21</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -672,7 +666,7 @@
         <v>13</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -683,8 +677,8 @@
       <c r="B14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>21</v>
+      <c r="C14" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
@@ -696,7 +690,7 @@
         <v>15</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
@@ -708,7 +702,7 @@
         <v>16</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -719,7 +713,7 @@
       <c r="B17" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -731,7 +725,7 @@
       <c r="B18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update the final test result
</commit_message>
<xml_diff>
--- a/tests/RealProjectCode.xlsx
+++ b/tests/RealProjectCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\exaba\maxio-driver-demo\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5793785-6308-45E5-BF38-1CD95CDE9EFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83CA235D-EDF6-44DD-A68B-A16DD90A556B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="39225" yWindow="0" windowWidth="24375" windowHeight="15330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
   <si>
     <t>Code</t>
   </si>
@@ -128,9 +128,6 @@
   </si>
   <si>
     <t>passed</t>
-  </si>
-  <si>
-    <t>failed</t>
   </si>
   <si>
     <t>$query-&gt;whereDoesntHave('status', function (Builder $query) {
@@ -148,7 +145,8 @@
             })</t>
   </si>
   <si>
-    <t>failed on test case 2</t>
+    <t>failed.
+Nested query is not supported yet.</t>
   </si>
 </sst>
 </file>
@@ -170,18 +168,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -202,7 +194,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -216,11 +208,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -504,8 +493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -642,7 +631,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
@@ -651,10 +640,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -665,8 +654,8 @@
       <c r="B13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>22</v>
+      <c r="C13" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -689,8 +678,8 @@
       <c r="B15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>20</v>
+      <c r="C15" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
@@ -701,8 +690,8 @@
       <c r="B16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>20</v>
+      <c r="C16" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>